<commit_message>
Lots of minor updates. Fixed bug when single user wouldn't show overview page. Added local users option.
</commit_message>
<xml_diff>
--- a/resources/guide.xlsx
+++ b/resources/guide.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28209"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jbryer/Dropbox (Personal)/Projects/DAACS-Github/student-dashboard/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alui\Google Drive\DAACS\Dashboard\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C099DF9-6C55-4A62-8737-99E0BA1ACBC6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14660" yWindow="460" windowWidth="23740" windowHeight="21140" tabRatio="500"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="19440" windowHeight="15600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="150000"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="60">
   <si>
     <t>Domain</t>
   </si>
@@ -41,39 +42,10 @@
     <t>Fixed Mindset</t>
   </si>
   <si>
-    <t>* View mistakes as a natural part 
-of learning.
-* Remind yourself that you can improve if 
-you just keep trying.</t>
-  </si>
-  <si>
-    <t>* http://srl.daacs.net/mindset.html
-* Dweck’s TED Talk:
-https://vimeo.com/207330839</t>
-  </si>
-  <si>
     <t>Poor Time Management</t>
   </si>
   <si>
-    <t>* Set aside regular times to study
-* Prioritize tasks 
-* Use a calendar</t>
-  </si>
-  <si>
-    <t>* http://srl.daacs.net/managing_time.html</t>
-  </si>
-  <si>
     <t>Poor Environment Management</t>
-  </si>
-  <si>
-    <t>* Set rules for others in your house about 
-“do not disturb” times
-* Turn off your cell phone
-* Identify comfortable and quiet places to 
-work</t>
-  </si>
-  <si>
-    <t>* http://srl.daacs.net/managing_environment.html</t>
   </si>
   <si>
     <t>Low Self-Efficacy</t>
@@ -96,120 +68,183 @@
 you do well in school.</t>
   </si>
   <si>
-    <t>* Watch the video at: http://srl.daacs.net/self-efficacy.html</t>
-  </si>
-  <si>
     <t>* Study over several short study sessions
 * Use practice quizzes or tests 
 * Use concept maps or make summaries.</t>
   </si>
   <si>
-    <t>* http://srl.daacs.net/understanding.html'</t>
-  </si>
-  <si>
-    <t>* Identify your area of weakness with 
-regard to planning, monitoring, 
-and evaluation</t>
-  </si>
-  <si>
-    <t>* Watch the video at: http://srl.daacs.net/metacognition.html</t>
+    <t>Challenge</t>
+  </si>
+  <si>
+    <t>mindset</t>
+  </si>
+  <si>
+    <t>managing_time</t>
+  </si>
+  <si>
+    <t>managing_environment</t>
+  </si>
+  <si>
+    <t>self_efficacy</t>
+  </si>
+  <si>
+    <t>mastery_orientation</t>
+  </si>
+  <si>
+    <t>anxiety</t>
+  </si>
+  <si>
+    <t>understanding</t>
+  </si>
+  <si>
+    <t>planning</t>
+  </si>
+  <si>
+    <t>monitoring</t>
+  </si>
+  <si>
+    <t>evaluation</t>
+  </si>
+  <si>
+    <t>Infrequent Metacognition (Planning)</t>
+  </si>
+  <si>
+    <t>Infrequent Metacognition (Monitoring)</t>
+  </si>
+  <si>
+    <t>Infrequent Metacognition (Evaluation)</t>
+  </si>
+  <si>
+    <t>Strength</t>
+  </si>
+  <si>
+    <t>Growth Mindset</t>
+  </si>
+  <si>
+    <t>Good Time Management</t>
+  </si>
+  <si>
+    <t>Good Environment Management</t>
+  </si>
+  <si>
+    <t>High Self-Efficacy</t>
+  </si>
+  <si>
+    <t>Good Strategies for Understanding</t>
+  </si>
+  <si>
+    <t>Frequent Metacognition (Planning)</t>
+  </si>
+  <si>
+    <t>Frequent Metacognition (Monitoring)</t>
+  </si>
+  <si>
+    <t>Frequent Metacongition (Evaluation)</t>
+  </si>
+  <si>
+    <t>Low Anxiety</t>
+  </si>
+  <si>
+    <t>* https://srl.daacs.net/motivation/mindset/
+* Dweck’s TED Talk:
+https://vimeo.com/207330839</t>
+  </si>
+  <si>
+    <t>* http://srl.daacs.net/learning-strategies/managing-time/</t>
+  </si>
+  <si>
+    <t>* http://srl.daacs.net/learning-strategies/managing-environment.html</t>
+  </si>
+  <si>
+    <t>* http://srl.daacs.net/learning-strategies/understanding.html'</t>
+  </si>
+  <si>
+    <t>* Watch the video at: https://srl.daacs.net/metacognition/plan/how-often-do-you-plan/</t>
+  </si>
+  <si>
+    <t>* Watch the video at: https://srl.daacs.net/metacognition/monitor/how-often-do-you-monitor/</t>
+  </si>
+  <si>
+    <t>* Watch the video at: https://srl.daacs.net/metacognition/evaluate/how-often-do-you-evaluate/</t>
+  </si>
+  <si>
+    <t>* https://srl.daacs.net/motivation/anxiety-levels/
+* Anxiety &amp; Depression Association of America: https://www.adaa.org/living-with-anxiety/children/test-anxiety</t>
+  </si>
+  <si>
+    <t>https://srl.daacs.net/motivation/mastery-orientation/</t>
+  </si>
+  <si>
+    <t>* Watch the video at: https://srl.daacs.net/motivation/self-efficacy/</t>
+  </si>
+  <si>
+    <t>*https://srl.daacs.net/learning-strategies/help-seeking/</t>
+  </si>
+  <si>
+    <t>* Identify the best sources of answers to your questions (Advisor? Instructor? Peer?)
+* Identify and write down the specific areas that give you trouble
+* Send an email, make a phonecall - reach out!</t>
+  </si>
+  <si>
+    <t>Infrequent Help-Seeking</t>
+  </si>
+  <si>
+    <t>Frequent Help-Seeking</t>
+  </si>
+  <si>
+    <t>help_seeking</t>
+  </si>
+  <si>
+    <t>* Set rules for others in your house about 
+“do not disturb” times
+* Turn off your cell phone or leave it in another room
+* Identify comfortable and quiet places to 
+work</t>
+  </si>
+  <si>
+    <t>* Here are some questions to ask yourself as you plan for an assignment:
+** How can I organize myself and my materials?
+** What do I already know, and what would I like to learn?
+** How much time do I have? How much time do I need?</t>
+  </si>
+  <si>
+    <t>* Here are some questions to ask yourself after you have completed an assignment:
+** What did I learn?
+** How well did I accomplish the goals of the assignment?
+** What should I do next teim?</t>
   </si>
   <si>
     <t>* Use relaxation techniques
-* Say positive things to yourself
+* Practice positive self-talk and challenge negative thoughts
 * Create schedules and plan study times</t>
   </si>
   <si>
-    <t>* http://srl.daacs.net/anxiety.html
-* Anxiety &amp; Depression Association of America: https://www.adaa.org/living-with-anxiety/children/test-anxiety</t>
-  </si>
-  <si>
-    <t>* Don't worry about how others perform
-* Focus on your improvement and 
-progress rather than a single grade.
+    <t>* Focus on your individual progress. If you must make comparisons, compare where you are today to where you were last week, or last semester.
+* Make learning relevant. Make connections between the course or assignment and your career, goals, or your life.
 * View mistakes and errors as opportunities 
 to improve.</t>
   </si>
   <si>
-    <t>http://srl.daacs.net/mastery_orientation.html</t>
-  </si>
-  <si>
-    <t>Challenge</t>
-  </si>
-  <si>
-    <t>mindset</t>
-  </si>
-  <si>
-    <t>managing_time</t>
-  </si>
-  <si>
-    <t>managing_environment</t>
-  </si>
-  <si>
-    <t>self_efficacy</t>
-  </si>
-  <si>
-    <t>mastery_orientation</t>
-  </si>
-  <si>
-    <t>anxiety</t>
-  </si>
-  <si>
-    <t>understanding</t>
-  </si>
-  <si>
-    <t>planning</t>
-  </si>
-  <si>
-    <t>monitoring</t>
-  </si>
-  <si>
-    <t>evaluation</t>
-  </si>
-  <si>
-    <t>Infrequent Metacognition (Planning)</t>
-  </si>
-  <si>
-    <t>Infrequent Metacognition (Monitoring)</t>
-  </si>
-  <si>
-    <t>Infrequent Metacognition (Evaluation)</t>
-  </si>
-  <si>
-    <t>Strength</t>
-  </si>
-  <si>
-    <t>Growth Mindset</t>
-  </si>
-  <si>
-    <t>Good Time Management</t>
-  </si>
-  <si>
-    <t>Good Environment Management</t>
-  </si>
-  <si>
-    <t>High Self-Efficacy</t>
-  </si>
-  <si>
-    <t>Good Strategies for Understanding</t>
-  </si>
-  <si>
-    <t>Frequent Metacognition (Planning)</t>
-  </si>
-  <si>
-    <t>Frequent Metacognition (Monitoring)</t>
-  </si>
-  <si>
-    <t>Frequent Metacongition (Evaluation)</t>
-  </si>
-  <si>
-    <t>Low Anxiety</t>
+    <t>* View mistakes as a natural part 
+of learning.
+* Embrace challenges, and ask for help when you are stuck</t>
+  </si>
+  <si>
+    <t>* Set aside regular times to study
+* Make a checklist and prioritize tasks
+* Use a calendar to keep track of deadlines</t>
+  </si>
+  <si>
+    <t>* Here are some questions to ask yourself while completing an assignment:
+** Am I meeting my learning goals? 
+** What strategies am I using and how are they working for me?
+** What other resources can I use to complete the assignment?</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -252,20 +287,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="3"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -273,6 +311,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -540,31 +581,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="21.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="21.625" customWidth="1"/>
     <col min="3" max="3" width="31" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="36.83203125" customWidth="1"/>
-    <col min="5" max="5" width="42.6640625" customWidth="1"/>
+    <col min="4" max="4" width="53.25" customWidth="1"/>
+    <col min="5" max="5" width="48.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>41</v>
+        <v>27</v>
       </c>
       <c r="C1" t="s">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -573,177 +614,197 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5" ht="64" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" t="s">
         <v>28</v>
-      </c>
-      <c r="B2" t="s">
-        <v>42</v>
       </c>
       <c r="C2" t="s">
         <v>3</v>
       </c>
       <c r="D2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="1" t="s">
+      <c r="D3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="E3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>29</v>
-      </c>
-      <c r="B3" t="s">
+      <c r="D4" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="E4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7" t="s">
+        <v>24</v>
+      </c>
+      <c r="D7" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B8" t="s">
+        <v>34</v>
+      </c>
+      <c r="C8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" t="s">
+        <v>35</v>
+      </c>
+      <c r="C9" t="s">
+        <v>26</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="C3" t="s">
-        <v>6</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" t="s">
+    </row>
+    <row r="10" spans="1:5" ht="63" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>19</v>
+      </c>
+      <c r="B10" t="s">
+        <v>36</v>
+      </c>
+      <c r="C10" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4" t="s">
+      <c r="D10" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="C4" t="s">
+    </row>
+    <row r="11" spans="1:5" ht="110.25" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>18</v>
+      </c>
+      <c r="B11" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="C11" t="s">
         <v>10</v>
       </c>
-      <c r="E4" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B5" t="s">
+      <c r="D11" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="E11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
-      <c r="D5" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E5" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>35</v>
-      </c>
-      <c r="B7" t="s">
+    </row>
+    <row r="12" spans="1:5" ht="94.5" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>51</v>
+      </c>
+      <c r="B12" t="s">
+        <v>50</v>
+      </c>
+      <c r="C12" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="E12" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C7" t="s">
-        <v>38</v>
-      </c>
-      <c r="D7" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B8" t="s">
-        <v>48</v>
-      </c>
-      <c r="C8" t="s">
-        <v>39</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E8" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5" ht="48" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
-        <v>37</v>
-      </c>
-      <c r="B9" t="s">
-        <v>49</v>
-      </c>
-      <c r="C9" t="s">
-        <v>40</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E9" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5" ht="64" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>33</v>
-      </c>
-      <c r="B10" t="s">
-        <v>50</v>
-      </c>
-      <c r="C10" t="s">
-        <v>14</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" ht="80" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
-        <v>32</v>
-      </c>
-      <c r="B11" t="s">
-        <v>15</v>
-      </c>
-      <c r="C11" t="s">
-        <v>16</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="E11" t="s">
-        <v>26</v>
-      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="E11" r:id="rId1" xr:uid="{40F77747-D0B0-4FB6-BF60-1264AC72ECB9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>